<commit_message>
excel descriptive analysis completed
</commit_message>
<xml_diff>
--- a/Statistical Analysis/Data+set+-+frequency+and+graphs.xlsx
+++ b/Statistical Analysis/Data+set+-+frequency+and+graphs.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\__Instructory Courses\# UDEMY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shubham-Data-Analytics\Data-Analytics-GitHub\Statistical Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F306E56-0C98-4AFF-96EB-8E7188929C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="765"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="765" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Basic Charts" sheetId="29" r:id="rId2"/>
+    <sheet name="Basics Charts" sheetId="30" r:id="rId2"/>
+    <sheet name="Descriptive Analysis" sheetId="31" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -24,17 +26,48 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="35">
   <si>
     <t>CGPA</t>
   </si>
@@ -63,12 +96,6 @@
     <t>Percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">Total </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bin </t>
-  </si>
-  <si>
     <t>Income (1=low, 2=medium, 3=high)</t>
   </si>
   <si>
@@ -89,12 +116,69 @@
   <si>
     <t>Low</t>
   </si>
+  <si>
+    <t>Frequency Distribution</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Bin</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Sample Variance</t>
+  </si>
+  <si>
+    <t>Kurtosis</t>
+  </si>
+  <si>
+    <t>Skewness</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Confidence Level(95.0%)</t>
+  </si>
+  <si>
+    <t>p.Mean Range</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,8 +207,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +231,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -167,47 +276,80 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -221,7 +363,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -235,7 +377,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -287,7 +428,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Charts'!$E$2:$E$3</c:f>
+              <c:f>'Basics Charts'!$E$3:$E$4</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -301,19 +442,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Charts'!$F$2:$F$3</c:f>
+              <c:f>'Basics Charts'!$F$3:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FEEC-4FD8-A7F5-2B3902712526}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -325,11 +471,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="302966224"/>
-        <c:axId val="210432072"/>
+        <c:axId val="1550417615"/>
+        <c:axId val="1550420495"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="302966224"/>
+        <c:axId val="1550417615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -372,7 +518,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210432072"/>
+        <c:crossAx val="1550420495"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -380,7 +526,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210432072"/>
+        <c:axId val="1550420495"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -431,7 +577,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302966224"/>
+        <c:crossAx val="1550417615"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -445,6 +591,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -481,7 +634,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -495,7 +648,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -621,14 +773,12 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Charts'!$E$2:$E$3</c:f>
+              <c:f>'Basics Charts'!$E$3:$E$4</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -642,19 +792,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Charts'!$F$2:$F$3</c:f>
+              <c:f>'Basics Charts'!$F$3:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A50E-4D9B-A1CD-9C496AE5BEBD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="inEnd"/>
@@ -678,7 +833,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -714,6 +868,13 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -757,7 +918,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -786,7 +947,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -812,7 +972,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Basic Charts'!$L$2:$L$12</c:f>
+              <c:f>'Basics Charts'!$M$3:$M$13</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -853,7 +1013,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Basic Charts'!$M$2:$M$12</c:f>
+              <c:f>'Basics Charts'!$N$3:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -893,6 +1053,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3891-4F00-BDD3-D62C16A58860}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -903,11 +1068,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="297187760"/>
-        <c:axId val="297185800"/>
+        <c:axId val="1550411855"/>
+        <c:axId val="1550407055"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="297187760"/>
+        <c:axId val="1550411855"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -924,19 +1089,18 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Bin </a:t>
+                  <a:t>Bin</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297185800"/>
+        <c:crossAx val="1550407055"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -944,7 +1108,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="297185800"/>
+        <c:axId val="1550407055"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -966,20 +1130,31 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297187760"/>
+        <c:crossAx val="1550411855"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
@@ -2108,20 +2283,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>517281</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>89073</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>911856</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>13246</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>753522</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>62696</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>692859</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>48633</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E84FD4C3-CDB1-AB05-13F1-71DCA88F4C61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2138,20 +2319,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>29255</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>207980</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>52498</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>172130</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>339986</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>24317</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7E7C661-A549-213B-828C-05D21F08DAD7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2168,20 +2355,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>274027</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>247651</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>167787</xdr:rowOff>
+      <xdr:rowOff>169546</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>274028</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>367889</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>167787</xdr:rowOff>
+      <xdr:rowOff>11205</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E2AEB96-2F12-2183-AFB1-4F51E9ABDC4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2461,482 +2654,570 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:F1048576"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="4" width="26.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="14.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="9.28515625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="13.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="1"/>
+    <col min="3" max="4" width="26.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="37.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="14.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875"/>
+    <col min="10" max="10" width="16.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="1"/>
+    <col min="14" max="14" width="9.33203125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3">
+        <f>IF(B2="Female",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" cm="1">
+        <f t="array" ref="E2">_xlfn.IFS(D2="High",3,D2="Medium",2,D2="Low",1)</f>
+        <v>3</v>
+      </c>
+      <c r="F2" s="3">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3">
+        <v>4</v>
+      </c>
+      <c r="H2" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:C16" si="0">IF(B3="Female",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E3" s="3" cm="1">
+        <f t="array" ref="E3">_xlfn.IFS(D3="High",3,D3="Medium",2,D3="Low",1)</f>
+        <v>2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4">
+        <v>3.55</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" cm="1">
+        <f t="array" ref="E4">_xlfn.IFS(D4="High",3,D4="Medium",2,D4="Low",1)</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3</v>
+      </c>
+      <c r="H4" s="4">
+        <v>3.35</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" cm="1">
+        <f t="array" ref="E5">_xlfn.IFS(D5="High",3,D5="Medium",2,D5="Low",1)</f>
+        <v>3</v>
+      </c>
+      <c r="F5" s="3">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3">
+        <v>7</v>
+      </c>
+      <c r="H5" s="4">
+        <v>3.65</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" cm="1">
+        <f t="array" ref="E6">_xlfn.IFS(D6="High",3,D6="Medium",2,D6="Low",1)</f>
+        <v>2</v>
+      </c>
+      <c r="F6" s="3">
+        <v>24</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2</v>
+      </c>
+      <c r="H6" s="4">
+        <v>3.25</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3" cm="1">
+        <f t="array" ref="E7">_xlfn.IFS(D7="High",3,D7="Medium",2,D7="Low",1)</f>
+        <v>3</v>
+      </c>
+      <c r="F7" s="3">
+        <v>23</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
+        <v>3</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3" cm="1">
+        <f t="array" ref="E8">_xlfn.IFS(D8="High",3,D8="Medium",2,D8="Low",1)</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>22</v>
+      </c>
+      <c r="G8" s="3">
+        <v>4</v>
+      </c>
+      <c r="H8" s="4">
+        <v>3.45</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="3" cm="1">
+        <f t="array" ref="E9">_xlfn.IFS(D9="High",3,D9="Medium",2,D9="Low",1)</f>
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>25</v>
+      </c>
+      <c r="G9" s="3">
+        <v>5</v>
+      </c>
+      <c r="H9" s="4">
+        <v>3.55</v>
+      </c>
+      <c r="N9" s="4"/>
+      <c r="O9"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="3" cm="1">
+        <f t="array" ref="E10">_xlfn.IFS(D10="High",3,D10="Medium",2,D10="Low",1)</f>
+        <v>2</v>
+      </c>
+      <c r="F10" s="3">
+        <v>21</v>
+      </c>
+      <c r="G10" s="3">
+        <v>6</v>
+      </c>
+      <c r="H10" s="4">
+        <v>3.65</v>
+      </c>
+      <c r="N10"/>
+      <c r="O10"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="3" cm="1">
+        <f t="array" ref="E11">_xlfn.IFS(D11="High",3,D11="Medium",2,D11="Low",1)</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>22</v>
+      </c>
+      <c r="G11" s="3">
+        <v>9</v>
+      </c>
+      <c r="H11" s="4">
+        <v>3.85</v>
+      </c>
+      <c r="N11"/>
+      <c r="O11"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="B12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="3" cm="1">
+        <f t="array" ref="E12">_xlfn.IFS(D12="High",3,D12="Medium",2,D12="Low",1)</f>
         <v>3</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="11" t="s">
+      <c r="F12" s="3">
+        <v>22</v>
+      </c>
+      <c r="G12" s="3">
+        <v>3</v>
+      </c>
+      <c r="H12" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="N12"/>
+      <c r="O12"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="D13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="3" cm="1">
+        <f t="array" ref="E13">_xlfn.IFS(D13="High",3,D13="Medium",2,D13="Low",1)</f>
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="F13" s="3">
+        <v>21</v>
+      </c>
+      <c r="G13" s="3">
         <v>5</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6">
-        <v>21</v>
-      </c>
-      <c r="G2" s="6">
-        <v>4</v>
-      </c>
-      <c r="H2" s="7">
-        <v>3.5</v>
-      </c>
-      <c r="L2" s="9"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6">
-        <v>22</v>
-      </c>
-      <c r="G3" s="6">
-        <v>5</v>
-      </c>
-      <c r="H3" s="7">
-        <v>3.55</v>
-      </c>
-      <c r="L3" s="9"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6">
-        <v>22</v>
-      </c>
-      <c r="G4" s="6">
-        <v>3</v>
-      </c>
-      <c r="H4" s="7">
-        <v>3.35</v>
-      </c>
-      <c r="L4" s="9"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6">
-        <v>20</v>
-      </c>
-      <c r="G5" s="6">
-        <v>7</v>
-      </c>
-      <c r="H5" s="7">
-        <v>3.65</v>
-      </c>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6">
-        <v>24</v>
-      </c>
-      <c r="G6" s="6">
-        <v>2</v>
-      </c>
-      <c r="H6" s="7">
-        <v>3.25</v>
-      </c>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6">
-        <v>23</v>
-      </c>
-      <c r="G7" s="6">
-        <v>1</v>
-      </c>
-      <c r="H7" s="7">
-        <v>3</v>
-      </c>
-      <c r="L7" s="9"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6">
-        <v>22</v>
-      </c>
-      <c r="G8" s="6">
-        <v>4</v>
-      </c>
-      <c r="H8" s="7">
-        <v>3.45</v>
-      </c>
-      <c r="L8" s="9"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6">
-        <v>25</v>
-      </c>
-      <c r="G9" s="6">
-        <v>5</v>
-      </c>
-      <c r="H9" s="7">
-        <v>3.55</v>
-      </c>
-      <c r="N9" s="7"/>
-      <c r="O9"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6">
-        <v>21</v>
-      </c>
-      <c r="G10" s="6">
-        <v>6</v>
-      </c>
-      <c r="H10" s="7">
-        <v>3.65</v>
-      </c>
-      <c r="N10" s="8"/>
-      <c r="O10"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6">
-        <v>22</v>
-      </c>
-      <c r="G11" s="6">
-        <v>9</v>
-      </c>
-      <c r="H11" s="7">
-        <v>3.85</v>
-      </c>
-      <c r="N11" s="8"/>
-      <c r="O11"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6">
-        <v>22</v>
-      </c>
-      <c r="G12" s="6">
-        <v>3</v>
-      </c>
-      <c r="H12" s="7">
-        <v>3.4</v>
-      </c>
-      <c r="N12" s="8"/>
-      <c r="O12"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6">
-        <v>21</v>
-      </c>
-      <c r="G13" s="6">
-        <v>5</v>
-      </c>
-      <c r="H13" s="7">
+      <c r="H13" s="4">
         <v>3.7</v>
       </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
       <c r="N13"/>
       <c r="O13"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6">
+      <c r="C14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="3" cm="1">
+        <f t="array" ref="E14">_xlfn.IFS(D14="High",3,D14="Medium",2,D14="Low",1)</f>
+        <v>2</v>
+      </c>
+      <c r="F14" s="3">
         <v>20</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="3">
         <v>6</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="4">
         <v>3.5</v>
       </c>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="5"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6" t="s">
+      <c r="C15" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="3" cm="1">
+        <f t="array" ref="E15">_xlfn.IFS(D15="High",3,D15="Medium",2,D15="Low",1)</f>
+        <v>3</v>
+      </c>
+      <c r="F15" s="3">
+        <v>23</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
+      <c r="H15" s="4">
+        <v>3.15</v>
+      </c>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6">
-        <v>23</v>
-      </c>
-      <c r="G15" s="6">
-        <v>3</v>
-      </c>
-      <c r="H15" s="7">
-        <v>3.15</v>
-      </c>
-      <c r="N15" s="6"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6">
+      <c r="C16" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="3" cm="1">
+        <f t="array" ref="E16">_xlfn.IFS(D16="High",3,D16="Medium",2,D16="Low",1)</f>
+        <v>2</v>
+      </c>
+      <c r="F16" s="3">
         <v>24</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="3">
         <v>4</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="4">
         <v>3.05</v>
       </c>
-      <c r="N16" s="7"/>
-    </row>
-    <row r="17" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H31" s="2"/>
-      <c r="J31" s="10"/>
-    </row>
-    <row r="32" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H32" s="2"/>
-      <c r="J32" s="10"/>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H33" s="13"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H18"/>
+    </row>
+    <row r="19" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H19"/>
+    </row>
+    <row r="20" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H20"/>
+    </row>
+    <row r="21" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H21"/>
+    </row>
+    <row r="22" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H22"/>
+    </row>
+    <row r="23" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H23"/>
+    </row>
+    <row r="24" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H24"/>
+    </row>
+    <row r="25" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H25"/>
+    </row>
+    <row r="26" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H26"/>
+    </row>
+    <row r="27" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H27"/>
+    </row>
+    <row r="28" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H28"/>
+    </row>
+    <row r="29" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H29"/>
+    </row>
+    <row r="30" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H30"/>
+    </row>
+    <row r="31" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H31"/>
+      <c r="J31" s="6"/>
+    </row>
+    <row r="32" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H32"/>
+      <c r="J32" s="6"/>
     </row>
   </sheetData>
-  <sortState ref="A2:H33">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H33">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2945,489 +3226,915 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABDBC2B-A5DE-4F8B-9342-AC41F926EF5F}">
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="16"/>
+    <col min="1" max="2" width="8.88671875" style="11"/>
+    <col min="3" max="3" width="27.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="11"/>
+    <col min="5" max="5" width="8.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="J1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3">
+        <f>IF(B2="Female",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="4" t="s">
+      <c r="J2" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="K2" s="4">
+        <v>3</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:C16" si="0">IF(B3="Female",0,1)</f>
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <f>IF(B2=B$2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1">
-        <f>COUNTIF(C2:C16,1)</f>
-        <v>8</v>
-      </c>
-      <c r="G2" s="9">
-        <f>F2/F4</f>
-        <v>0.53333333333333333</v>
-      </c>
-      <c r="I2" s="7">
-        <v>3.5</v>
-      </c>
-      <c r="J2" s="6">
+      <c r="F3" s="11">
+        <f>COUNTIF(B2:B16,"Female")</f>
+        <v>7</v>
+      </c>
+      <c r="G3" s="13">
+        <f>F3/$F$5</f>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="J3" s="4">
+        <v>3.55</v>
+      </c>
+      <c r="K3" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="M3" s="15">
         <v>3</v>
       </c>
-      <c r="L2" s="15">
+      <c r="N3" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="M2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C16" si="0">IF(B3=B$2,0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1">
-        <f>COUNTIF(C2:C16,0)</f>
-        <v>7</v>
-      </c>
-      <c r="G3" s="9">
-        <f>F3/F4</f>
-        <v>0.46666666666666667</v>
-      </c>
-      <c r="I3" s="7">
-        <v>3.55</v>
-      </c>
-      <c r="J3" s="6">
-        <v>3.1</v>
-      </c>
-      <c r="L3" s="15">
-        <v>3.1</v>
-      </c>
-      <c r="M3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1">
-        <f>SUM(F2:F3)</f>
-        <v>15</v>
-      </c>
-      <c r="G4" s="9">
-        <f>F4/15</f>
+      <c r="E4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="11">
+        <f>COUNTIF(B2:B16,"Male")</f>
+        <v>8</v>
+      </c>
+      <c r="G4" s="13">
+        <f>F4/$F$5</f>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="J4" s="4">
+        <v>3.35</v>
+      </c>
+      <c r="K4" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="M4" s="15">
+        <v>3.1</v>
+      </c>
+      <c r="N4" s="16">
         <v>1</v>
       </c>
-      <c r="I4" s="7">
-        <v>3.35</v>
-      </c>
-      <c r="J4" s="6">
-        <v>3.2</v>
-      </c>
-      <c r="L4" s="15">
-        <v>3.2</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+    </row>
+    <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I5" s="7">
+      <c r="E5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="11">
+        <f>SUM(F3:F4)</f>
+        <v>15</v>
+      </c>
+      <c r="G5" s="13">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4">
         <v>3.65</v>
       </c>
-      <c r="J5" s="6">
+      <c r="K5" s="4">
         <v>3.3</v>
       </c>
-      <c r="L5" s="15">
-        <v>3.3</v>
-      </c>
-      <c r="M5" s="2">
+      <c r="M5" s="15">
+        <v>3.2</v>
+      </c>
+      <c r="N5" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I6" s="7">
+      <c r="J6" s="4">
         <v>3.25</v>
       </c>
-      <c r="J6" s="6">
+      <c r="K6" s="4">
         <v>3.4</v>
       </c>
-      <c r="L6" s="15">
-        <v>3.4</v>
-      </c>
-      <c r="M6" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="M6" s="15">
+        <v>3.3</v>
+      </c>
+      <c r="N6" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I7" s="17">
+      <c r="J7" s="4">
         <v>3</v>
       </c>
-      <c r="J7" s="6">
+      <c r="K7" s="4">
         <v>3.5</v>
       </c>
-      <c r="L7" s="15">
-        <v>3.5</v>
-      </c>
-      <c r="M7" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="M7" s="15">
+        <v>3.4</v>
+      </c>
+      <c r="N7" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="7">
+      <c r="J8" s="4">
         <v>3.45</v>
       </c>
-      <c r="J8" s="6">
+      <c r="K8" s="4">
         <v>3.6</v>
       </c>
-      <c r="L8" s="15">
-        <v>3.6</v>
-      </c>
-      <c r="M8" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="M8" s="15">
+        <v>3.5</v>
+      </c>
+      <c r="N8" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I9" s="7">
+      <c r="J9" s="4">
         <v>3.55</v>
       </c>
-      <c r="J9" s="6">
+      <c r="K9" s="4">
         <v>3.7</v>
       </c>
-      <c r="L9" s="15">
-        <v>3.7</v>
-      </c>
-      <c r="M9" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="M9" s="15">
+        <v>3.6</v>
+      </c>
+      <c r="N9" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="7">
+      <c r="J10" s="4">
         <v>3.65</v>
       </c>
-      <c r="J10" s="6">
+      <c r="K10" s="4">
         <v>3.8</v>
       </c>
-      <c r="L10" s="15">
-        <v>3.8</v>
-      </c>
-      <c r="M10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="M10" s="15">
+        <v>3.7</v>
+      </c>
+      <c r="N10" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="17">
+      <c r="J11" s="4">
         <v>3.85</v>
       </c>
-      <c r="J11" s="6">
+      <c r="K11" s="4">
         <v>3.9</v>
       </c>
-      <c r="L11" s="15">
-        <v>3.9</v>
-      </c>
-      <c r="M11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+      <c r="M11" s="15">
+        <v>3.8</v>
+      </c>
+      <c r="N11" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I12" s="7">
+      <c r="J12" s="4">
         <v>3.4</v>
       </c>
-      <c r="J12" s="6"/>
-      <c r="L12" s="3" t="s">
+      <c r="M12" s="15">
+        <v>3.9</v>
+      </c>
+      <c r="N12" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="M12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="7">
+      <c r="J13" s="4">
         <v>3.7</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="M13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="N13" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="7">
+      <c r="J14" s="4">
         <v>3.5</v>
       </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+    </row>
+    <row r="15" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I15" s="7">
+      <c r="J15" s="4">
         <v>3.15</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+    <row r="16" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I16" s="7">
+      <c r="J16" s="4">
         <v>3.05</v>
       </c>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-    </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-    </row>
   </sheetData>
-  <sortState ref="L2:L11">
-    <sortCondition ref="L2"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M3:M12">
+    <sortCondition ref="M3"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="J2:J16">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>3.85</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49149C60-A919-4D09-87D0-356EEC409E09}">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3.55</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="21">
+        <v>22.133333333333333</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="21">
+        <v>4.4666666666666668</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="21">
+        <v>3.4399999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3.35</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="20">
+        <v>0.37628088124073156</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="20">
+        <v>0.52432874699050691</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="20">
+        <v>6.290582530372571E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3.65</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="20">
+        <v>22</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="20">
+        <v>4</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="20">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3.25</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="20">
+        <v>22</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="20">
+        <v>4</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="20">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="21">
+        <v>1.4573295865416043</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="21">
+        <v>2.0307165050320357</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="21">
+        <v>0.2436332137807628</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3.45</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="20">
+        <v>2.1238095238095234</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="20">
+        <v>4.1238095238095251</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="20">
+        <v>5.9357142857142865E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3.55</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="21">
+        <v>-0.37502494288272947</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="21">
+        <v>0.56222990723147959</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="21">
+        <v>-0.46013926469817035</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3.65</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="21">
+        <v>0.37469242869740704</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="21">
+        <v>0.49847329619568087</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="21">
+        <v>-0.38999310504777251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3.85</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="20">
+        <v>5</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="20">
+        <v>8</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" s="20">
+        <v>0.85000000000000009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="20">
+        <v>20</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="20">
+        <v>1</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="C13" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="20">
+        <v>25</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="20">
+        <v>9</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="20">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="20">
+        <v>332</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="20">
+        <v>67</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="20">
+        <v>51.599999999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>23</v>
+      </c>
+      <c r="B15" s="3">
+        <v>3</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3.15</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="20">
+        <v>15</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="20">
+        <v>15</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15" s="20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
+        <v>24</v>
+      </c>
+      <c r="B16" s="3">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4">
+        <v>3.05</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="22">
+        <v>0.80704222500310097</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="22">
+        <v>1.1245733166378613</v>
+      </c>
+      <c r="J16" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="22">
+        <v>0.13491957670391383</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="23">
+        <f>G3-G16</f>
+        <v>21.326291108330231</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="G20" s="23">
+        <f>G3+G16</f>
+        <v>22.940375558336434</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>